<commit_message>
Working on Soil Moisture Deficit
</commit_message>
<xml_diff>
--- a/TrialData.xlsx
+++ b/TrialData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\NBR\20. NBR\780 5T Growth model\780_growth_model\clone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\NBR\20. NBR\905 Nordic Beet Yield Challenge NBYC\clone\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>TrialID</t>
   </si>
@@ -129,6 +129,15 @@
   </si>
   <si>
     <t>Can2bLOS</t>
+  </si>
+  <si>
+    <t>SowDate</t>
+  </si>
+  <si>
+    <t>HarvestDate</t>
+  </si>
+  <si>
+    <t>EmDate</t>
   </si>
 </sst>
 </file>
@@ -164,8 +173,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,15 +456,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI8"/>
+  <dimension ref="A1:AL8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,94 +487,103 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -580,44 +602,44 @@
       <c r="F2">
         <v>2.4</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
+        <v>42095</v>
+      </c>
+      <c r="H2" s="1">
+        <v>42309</v>
+      </c>
+      <c r="I2" s="1">
+        <v>42119</v>
+      </c>
+      <c r="J2">
         <v>104</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>319</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>114</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -667,8 +689,17 @@
       <c r="AI2">
         <v>0</v>
       </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -687,44 +718,44 @@
       <c r="F3">
         <v>2.4</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
+        <v>42461</v>
+      </c>
+      <c r="H3" s="1">
+        <v>42675</v>
+      </c>
+      <c r="I3" s="1">
+        <v>42485</v>
+      </c>
+      <c r="J3">
         <v>94</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>319</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>104</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -774,8 +805,17 @@
       <c r="AI3">
         <v>0</v>
       </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -794,44 +834,44 @@
       <c r="F4">
         <v>2.4</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
+        <v>42826</v>
+      </c>
+      <c r="H4" s="1">
+        <v>43040</v>
+      </c>
+      <c r="I4" s="1">
+        <v>42850</v>
+      </c>
+      <c r="J4">
         <v>103</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>319</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>113</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -881,8 +921,17 @@
       <c r="AI4">
         <v>0</v>
       </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -901,44 +950,44 @@
       <c r="F5">
         <v>2.4</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
+        <v>43191</v>
+      </c>
+      <c r="H5" s="1">
+        <v>43405</v>
+      </c>
+      <c r="I5" s="1">
+        <v>43215</v>
+      </c>
+      <c r="J5">
         <v>107</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>319</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <v>117</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -988,8 +1037,17 @@
       <c r="AI5">
         <v>0</v>
       </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1008,44 +1066,44 @@
       <c r="F6">
         <v>2.4</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
+        <v>43556</v>
+      </c>
+      <c r="H6" s="1">
+        <v>43770</v>
+      </c>
+      <c r="I6" s="1">
+        <v>43580</v>
+      </c>
+      <c r="J6">
         <v>97</v>
       </c>
-      <c r="H6">
+      <c r="K6">
         <v>319</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>107</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -1095,8 +1153,17 @@
       <c r="AI6">
         <v>0</v>
       </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1115,44 +1182,44 @@
       <c r="F7">
         <v>2.4</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
+        <v>43922</v>
+      </c>
+      <c r="H7" s="1">
+        <v>44136</v>
+      </c>
+      <c r="I7" s="1">
+        <v>43946</v>
+      </c>
+      <c r="J7">
         <v>94</v>
       </c>
-      <c r="H7">
+      <c r="K7">
         <v>319</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <v>104</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -1202,8 +1269,17 @@
       <c r="AI7">
         <v>0</v>
       </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1222,44 +1298,44 @@
       <c r="F8">
         <v>2.4</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
+        <v>44287</v>
+      </c>
+      <c r="H8" s="1">
+        <v>44501</v>
+      </c>
+      <c r="I8" s="1">
+        <v>44311</v>
+      </c>
+      <c r="J8">
         <v>104</v>
       </c>
-      <c r="H8">
+      <c r="K8">
         <v>319</v>
       </c>
-      <c r="I8">
+      <c r="L8">
         <v>114</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="P8">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -1307,6 +1383,15 @@
         <v>0</v>
       </c>
       <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improving system flow. Now imports weather from Lantmet, transforms, saves for model.
</commit_message>
<xml_diff>
--- a/TrialData.xlsx
+++ b/TrialData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>TrialID</t>
   </si>
@@ -44,15 +44,6 @@
     <t>SoilB</t>
   </si>
   <si>
-    <t>SowDOY</t>
-  </si>
-  <si>
-    <t>HarvestDOY</t>
-  </si>
-  <si>
-    <t>EmDOY</t>
-  </si>
-  <si>
     <t>Emergence</t>
   </si>
   <si>
@@ -138,6 +129,12 @@
   </si>
   <si>
     <t>EmDate</t>
+  </si>
+  <si>
+    <t>Weather_source</t>
+  </si>
+  <si>
+    <t>Lantmet</t>
   </si>
 </sst>
 </file>
@@ -456,18 +453,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL8"/>
+  <dimension ref="A1:AK8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,97 +488,94 @@
         <v>36</v>
       </c>
       <c r="I1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -602,23 +594,23 @@
       <c r="F2">
         <v>2.4</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2">
+        <v>40141</v>
+      </c>
+      <c r="I2" s="1">
         <v>42095</v>
       </c>
-      <c r="H2" s="1">
+      <c r="J2" s="1">
         <v>42309</v>
       </c>
-      <c r="I2" s="1">
+      <c r="K2" s="1">
         <v>42119</v>
       </c>
-      <c r="J2">
-        <v>104</v>
-      </c>
-      <c r="K2">
-        <v>319</v>
-      </c>
       <c r="L2">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -630,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="Q2">
         <v>90000</v>
@@ -639,7 +631,7 @@
         <v>90000</v>
       </c>
       <c r="S2">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -695,11 +687,8 @@
       <c r="AK2">
         <v>0</v>
       </c>
-      <c r="AL2">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -718,23 +707,23 @@
       <c r="F3">
         <v>2.4</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3">
+        <v>40141</v>
+      </c>
+      <c r="I3" s="1">
         <v>42461</v>
       </c>
-      <c r="H3" s="1">
+      <c r="J3" s="1">
         <v>42675</v>
       </c>
-      <c r="I3" s="1">
+      <c r="K3" s="1">
         <v>42485</v>
       </c>
-      <c r="J3">
-        <v>94</v>
-      </c>
-      <c r="K3">
-        <v>319</v>
-      </c>
       <c r="L3">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -746,7 +735,7 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="Q3">
         <v>90000</v>
@@ -755,7 +744,7 @@
         <v>90000</v>
       </c>
       <c r="S3">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -811,11 +800,8 @@
       <c r="AK3">
         <v>0</v>
       </c>
-      <c r="AL3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -834,23 +820,23 @@
       <c r="F4">
         <v>2.4</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4">
+        <v>40141</v>
+      </c>
+      <c r="I4" s="1">
         <v>42826</v>
       </c>
-      <c r="H4" s="1">
+      <c r="J4" s="1">
         <v>43040</v>
       </c>
-      <c r="I4" s="1">
+      <c r="K4" s="1">
         <v>42850</v>
       </c>
-      <c r="J4">
-        <v>103</v>
-      </c>
-      <c r="K4">
-        <v>319</v>
-      </c>
       <c r="L4">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -862,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="Q4">
         <v>90000</v>
@@ -871,7 +857,7 @@
         <v>90000</v>
       </c>
       <c r="S4">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -927,11 +913,8 @@
       <c r="AK4">
         <v>0</v>
       </c>
-      <c r="AL4">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -950,23 +933,23 @@
       <c r="F5">
         <v>2.4</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5">
+        <v>40141</v>
+      </c>
+      <c r="I5" s="1">
         <v>43191</v>
       </c>
-      <c r="H5" s="1">
+      <c r="J5" s="1">
         <v>43405</v>
       </c>
-      <c r="I5" s="1">
+      <c r="K5" s="1">
         <v>43215</v>
       </c>
-      <c r="J5">
-        <v>107</v>
-      </c>
-      <c r="K5">
-        <v>319</v>
-      </c>
       <c r="L5">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -978,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="Q5">
         <v>90000</v>
@@ -987,7 +970,7 @@
         <v>90000</v>
       </c>
       <c r="S5">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -1043,11 +1026,8 @@
       <c r="AK5">
         <v>0</v>
       </c>
-      <c r="AL5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1066,23 +1046,23 @@
       <c r="F6">
         <v>2.4</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6">
+        <v>40141</v>
+      </c>
+      <c r="I6" s="1">
         <v>43556</v>
       </c>
-      <c r="H6" s="1">
+      <c r="J6" s="1">
         <v>43770</v>
       </c>
-      <c r="I6" s="1">
+      <c r="K6" s="1">
         <v>43580</v>
       </c>
-      <c r="J6">
-        <v>97</v>
-      </c>
-      <c r="K6">
-        <v>319</v>
-      </c>
       <c r="L6">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1094,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="Q6">
         <v>90000</v>
@@ -1103,7 +1083,7 @@
         <v>90000</v>
       </c>
       <c r="S6">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -1159,11 +1139,8 @@
       <c r="AK6">
         <v>0</v>
       </c>
-      <c r="AL6">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1182,23 +1159,23 @@
       <c r="F7">
         <v>2.4</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7">
+        <v>40141</v>
+      </c>
+      <c r="I7" s="1">
         <v>43922</v>
       </c>
-      <c r="H7" s="1">
+      <c r="J7" s="1">
         <v>44136</v>
       </c>
-      <c r="I7" s="1">
+      <c r="K7" s="1">
         <v>43946</v>
       </c>
-      <c r="J7">
-        <v>94</v>
-      </c>
-      <c r="K7">
-        <v>319</v>
-      </c>
       <c r="L7">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1210,7 +1187,7 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="Q7">
         <v>90000</v>
@@ -1219,7 +1196,7 @@
         <v>90000</v>
       </c>
       <c r="S7">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -1275,11 +1252,8 @@
       <c r="AK7">
         <v>0</v>
       </c>
-      <c r="AL7">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1298,23 +1272,23 @@
       <c r="F8">
         <v>2.4</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8">
+        <v>40141</v>
+      </c>
+      <c r="I8" s="1">
         <v>44287</v>
       </c>
-      <c r="H8" s="1">
+      <c r="J8" s="1">
         <v>44501</v>
       </c>
-      <c r="I8" s="1">
+      <c r="K8" s="1">
         <v>44311</v>
       </c>
-      <c r="J8">
-        <v>104</v>
-      </c>
-      <c r="K8">
-        <v>319</v>
-      </c>
       <c r="L8">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1326,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="Q8">
         <v>90000</v>
@@ -1335,7 +1309,7 @@
         <v>90000</v>
       </c>
       <c r="S8">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -1389,9 +1363,6 @@
         <v>0</v>
       </c>
       <c r="AK8">
-        <v>0</v>
-      </c>
-      <c r="AL8">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Model looks to be working the same as OM, when the same input data is used.
</commit_message>
<xml_diff>
--- a/TrialData.xlsx
+++ b/TrialData.xlsx
@@ -99,15 +99,6 @@
     <t>weather_source_info</t>
   </si>
   <si>
-    <t>sow_date</t>
-  </si>
-  <si>
-    <t>harvest_date</t>
-  </si>
-  <si>
-    <t>em_date</t>
-  </si>
-  <si>
     <t>plant_pop</t>
   </si>
   <si>
@@ -175,6 +166,15 @@
   </si>
   <si>
     <t>can2blos</t>
+  </si>
+  <si>
+    <t>date_sow</t>
+  </si>
+  <si>
+    <t>date_harvest</t>
+  </si>
+  <si>
+    <t>date_emerg</t>
   </si>
 </sst>
 </file>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -545,19 +545,19 @@
         <v>23</v>
       </c>
       <c r="N1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="O1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="P1" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="Q1" t="s">
         <v>12</v>
       </c>
       <c r="R1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="S1" t="s">
         <v>13</v>
@@ -566,75 +566,75 @@
         <v>14</v>
       </c>
       <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
         <v>28</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA1" t="s">
         <v>29</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AB1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AE1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AH1" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AI1" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AK1" t="s">
         <v>39</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AL1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AM1" t="s">
         <v>33</v>
       </c>
-      <c r="AE1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="AN1" t="s">
         <v>45</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AO1" t="s">
         <v>34</v>
       </c>
-      <c r="AH1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI1" t="s">
+      <c r="AP1" t="s">
         <v>46</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A2">
-        <f>C2*10000+E2+G2*100-200000</f>
+        <f t="shared" ref="A2:A8" si="0">C2*10000+E2+G2*100-200000</f>
         <v>11501</v>
       </c>
       <c r="B2">
@@ -683,7 +683,7 @@
         <v>42309</v>
       </c>
       <c r="P2" s="1">
-        <v>42119</v>
+        <v>42118</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A3">
-        <f>C3*10000+E3+G3*100-200000</f>
+        <f t="shared" si="0"/>
         <v>11601</v>
       </c>
       <c r="B3">
@@ -898,7 +898,7 @@
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A4">
-        <f>C4*10000+E4+G4*100-200000</f>
+        <f t="shared" si="0"/>
         <v>11701</v>
       </c>
       <c r="B4">
@@ -1030,7 +1030,7 @@
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A5">
-        <f>C5*10000+E5+G5*100-200000</f>
+        <f t="shared" si="0"/>
         <v>11801</v>
       </c>
       <c r="B5">
@@ -1162,7 +1162,7 @@
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A6">
-        <f>C6*10000+E6+G6*100-200000</f>
+        <f t="shared" si="0"/>
         <v>11901</v>
       </c>
       <c r="B6">
@@ -1294,7 +1294,7 @@
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A7">
-        <f>C7*10000+E7+G7*100-200000</f>
+        <f t="shared" si="0"/>
         <v>12001</v>
       </c>
       <c r="B7">
@@ -1426,7 +1426,7 @@
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A8">
-        <f>C8*10000+E8+G8*100-200000</f>
+        <f t="shared" si="0"/>
         <v>12101</v>
       </c>
       <c r="B8">

</xml_diff>